<commit_message>
This is iNeuron Assignment
</commit_message>
<xml_diff>
--- a/Assignment5/Slicer_Assignment/Project_Plan_Datasets.xlsx
+++ b/Assignment5/Slicer_Assignment/Project_Plan_Datasets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://4lbi-my.sharepoint.com/personal/shannon_4lbi_com/Documents/Public/WOW/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\FSDA_Assignment\Assignment5\Slicer_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E55C4DF8-FA8D-4D56-B27A-398C7C08507C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE702C97-1D92-4F69-8CDD-9741152C1A09}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38510" yWindow="-10260" windowWidth="38620" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1400" yWindow="1400" windowWidth="19360" windowHeight="11930" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tasks" sheetId="1" r:id="rId1"/>
@@ -24,12 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -37,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="386" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="91">
   <si>
     <t>Task ID</t>
   </si>
@@ -114,15 +111,9 @@
     <t/>
   </si>
   <si>
-    <t>02/01/2022</t>
-  </si>
-  <si>
     <t>false</t>
   </si>
   <si>
-    <t>03/19/2022</t>
-  </si>
-  <si>
     <t>0/3</t>
   </si>
   <si>
@@ -141,9 +132,6 @@
     <t>Joni Sherman</t>
   </si>
   <si>
-    <t>02/04/2022</t>
-  </si>
-  <si>
     <t>0/2</t>
   </si>
   <si>
@@ -168,9 +156,6 @@
     <t>Lee Gu</t>
   </si>
   <si>
-    <t>03/25/2022</t>
-  </si>
-  <si>
     <t>1/3</t>
   </si>
   <si>
@@ -192,9 +177,6 @@
     <t>Joni Sherman;Diego Siciliani</t>
   </si>
   <si>
-    <t>03/26/2022</t>
-  </si>
-  <si>
     <t>e-AOJrIk90WIGQ1KnGAjs2UAHIx1</t>
   </si>
   <si>
@@ -207,36 +189,21 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>03/20/2022</t>
-  </si>
-  <si>
-    <t>04/15/2022</t>
-  </si>
-  <si>
     <t>ljVI_v5b10mfFzF3RSVh8GUAFU-D</t>
   </si>
   <si>
     <t>Task 4</t>
   </si>
   <si>
-    <t>04/01/2022</t>
-  </si>
-  <si>
     <t>hVuj4Isyi0eL_hitW6mSZ2UAPWmz</t>
   </si>
   <si>
     <t>Task</t>
   </si>
   <si>
-    <t>04/11/2022</t>
-  </si>
-  <si>
     <t>assidjJTCkyIfsWK4uh2_GUANyg8</t>
   </si>
   <si>
-    <t>03/23/2022</t>
-  </si>
-  <si>
     <t>Z2cdySLS30SrLfk8tQMikWUAAurZ</t>
   </si>
   <si>
@@ -246,24 +213,15 @@
     <t>Create outstanding videos</t>
   </si>
   <si>
-    <t>04/29/2022</t>
-  </si>
-  <si>
     <t>DQlxxxRXDUuJX4W3NJM4ImUADyEI</t>
   </si>
   <si>
     <t xml:space="preserve">Task </t>
   </si>
   <si>
-    <t>05/02/2022</t>
-  </si>
-  <si>
     <t>s4PVKsrlCU6qF0zrzRyl-GUABoV6</t>
   </si>
   <si>
-    <t>03/14/2022</t>
-  </si>
-  <si>
     <t>true</t>
   </si>
   <si>
@@ -273,9 +231,6 @@
     <t>V51QdIjVQEugA4lZXdXGOGUAHfOb</t>
   </si>
   <si>
-    <t>03/07/2022</t>
-  </si>
-  <si>
     <t>Subtask 3;Subtask 1;Subtask 2</t>
   </si>
   <si>
@@ -306,9 +261,6 @@
     <t>E3-vDpa570-XiPBIeGHLOWUAJyjJ</t>
   </si>
   <si>
-    <t>03/14/2021</t>
-  </si>
-  <si>
     <t>CbBnd50F0kq2rDvdOMXIuWUANxg-</t>
   </si>
   <si>
@@ -328,13 +280,40 @@
   </si>
   <si>
     <t>Date of export</t>
+  </si>
+  <si>
+    <t>03-20-2022</t>
+  </si>
+  <si>
+    <t>03-25-2022</t>
+  </si>
+  <si>
+    <t>03-26-2022</t>
+  </si>
+  <si>
+    <t>04-15-2022</t>
+  </si>
+  <si>
+    <t>03-23-2022</t>
+  </si>
+  <si>
+    <t>04-29-2022</t>
+  </si>
+  <si>
+    <t>03-14-2022</t>
+  </si>
+  <si>
+    <t>03-14-2021</t>
+  </si>
+  <si>
+    <t>03-19-2022</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -713,29 +692,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.875" customWidth="1"/>
-    <col min="2" max="2" width="24.875" customWidth="1"/>
-    <col min="3" max="3" width="18.875" customWidth="1"/>
-    <col min="4" max="4" width="14.875" customWidth="1"/>
-    <col min="5" max="5" width="18.875" customWidth="1"/>
-    <col min="6" max="6" width="24.875" customWidth="1"/>
-    <col min="7" max="7" width="18.875" customWidth="1"/>
-    <col min="8" max="10" width="11.875" customWidth="1"/>
-    <col min="11" max="11" width="8.875" customWidth="1"/>
-    <col min="12" max="12" width="11.875" customWidth="1"/>
-    <col min="13" max="13" width="18.875" customWidth="1"/>
-    <col min="14" max="14" width="32.875" customWidth="1"/>
-    <col min="15" max="15" width="8.875" customWidth="1"/>
-    <col min="16" max="17" width="32.875" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" customWidth="1"/>
+    <col min="2" max="2" width="24.83203125" customWidth="1"/>
+    <col min="3" max="3" width="18.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" customWidth="1"/>
+    <col min="5" max="5" width="18.83203125" customWidth="1"/>
+    <col min="6" max="6" width="24.83203125" customWidth="1"/>
+    <col min="7" max="7" width="18.83203125" customWidth="1"/>
+    <col min="8" max="10" width="11.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" customWidth="1"/>
+    <col min="12" max="12" width="11.83203125" customWidth="1"/>
+    <col min="13" max="13" width="18.83203125" customWidth="1"/>
+    <col min="14" max="14" width="32.83203125" customWidth="1"/>
+    <col min="15" max="15" width="8.83203125" customWidth="1"/>
+    <col min="16" max="17" width="32.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -788,7 +767,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -816,37 +795,37 @@
       <c r="I2" t="s">
         <v>24</v>
       </c>
-      <c r="J2" t="s">
-        <v>25</v>
+      <c r="J2" s="1">
+        <v>44563</v>
       </c>
       <c r="K2" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" t="s">
+        <v>90</v>
+      </c>
+      <c r="M2" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" t="s">
+        <v>24</v>
+      </c>
+      <c r="O2" t="s">
         <v>26</v>
       </c>
-      <c r="L2" t="s">
+      <c r="P2" t="s">
         <v>27</v>
       </c>
-      <c r="M2" t="s">
-        <v>22</v>
-      </c>
-      <c r="N2" t="s">
-        <v>24</v>
-      </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>28</v>
       </c>
-      <c r="P2" t="s">
+      <c r="B3" t="s">
         <v>29</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3" t="s">
-        <v>31</v>
       </c>
       <c r="C3" t="s">
         <v>19</v>
@@ -855,10 +834,10 @@
         <v>20</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G3" t="s">
         <v>22</v>
@@ -869,11 +848,11 @@
       <c r="I3" t="s">
         <v>24</v>
       </c>
-      <c r="J3" t="s">
-        <v>34</v>
+      <c r="J3" s="1">
+        <v>44653</v>
       </c>
       <c r="K3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L3" s="1">
         <v>44609</v>
@@ -885,33 +864,33 @@
         <v>24</v>
       </c>
       <c r="O3" t="s">
+        <v>32</v>
+      </c>
+      <c r="P3" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" t="s">
         <v>35</v>
       </c>
-      <c r="P3" t="s">
+      <c r="C4" t="s">
         <v>36</v>
       </c>
-      <c r="Q3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17">
-      <c r="A4" t="s">
+      <c r="D4" t="s">
         <v>37</v>
       </c>
-      <c r="B4" t="s">
+      <c r="E4" t="s">
         <v>38</v>
       </c>
-      <c r="C4" t="s">
+      <c r="F4" t="s">
         <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>40</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>42</v>
       </c>
       <c r="G4" t="s">
         <v>22</v>
@@ -923,48 +902,48 @@
         <v>44621</v>
       </c>
       <c r="J4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K4" t="s">
+        <v>25</v>
+      </c>
+      <c r="L4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N4" t="s">
+        <v>24</v>
+      </c>
+      <c r="O4" t="s">
+        <v>40</v>
+      </c>
+      <c r="P4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
-        <v>26</v>
-      </c>
-      <c r="L4" t="s">
-        <v>24</v>
-      </c>
-      <c r="M4" t="s">
-        <v>24</v>
-      </c>
-      <c r="N4" t="s">
-        <v>24</v>
-      </c>
-      <c r="O4" t="s">
+      <c r="C5" t="s">
         <v>44</v>
       </c>
-      <c r="P4" t="s">
+      <c r="D5" t="s">
         <v>45</v>
       </c>
-      <c r="Q4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17">
-      <c r="A5" t="s">
+      <c r="E5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" t="s">
         <v>46</v>
-      </c>
-      <c r="B5" t="s">
-        <v>47</v>
-      </c>
-      <c r="C5" t="s">
-        <v>48</v>
-      </c>
-      <c r="D5" t="s">
-        <v>49</v>
-      </c>
-      <c r="E5" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" t="s">
-        <v>50</v>
       </c>
       <c r="G5" t="s">
         <v>23</v>
@@ -976,169 +955,169 @@
         <v>24</v>
       </c>
       <c r="J5" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L5" t="s">
+        <v>24</v>
+      </c>
+      <c r="M5" t="s">
+        <v>24</v>
+      </c>
+      <c r="N5" t="s">
+        <v>24</v>
+      </c>
+      <c r="O5" t="s">
+        <v>40</v>
+      </c>
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E6" t="s">
+        <v>50</v>
+      </c>
+      <c r="F6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" t="s">
+        <v>22</v>
+      </c>
+      <c r="H6" t="s">
+        <v>82</v>
+      </c>
+      <c r="I6" t="s">
+        <v>24</v>
+      </c>
+      <c r="J6" t="s">
+        <v>85</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N6" t="s">
+        <v>24</v>
+      </c>
+      <c r="O6" t="s">
+        <v>24</v>
+      </c>
+      <c r="P6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>51</v>
       </c>
-      <c r="K5" t="s">
-        <v>26</v>
-      </c>
-      <c r="L5" t="s">
-        <v>24</v>
-      </c>
-      <c r="M5" t="s">
-        <v>24</v>
-      </c>
-      <c r="N5" t="s">
-        <v>24</v>
-      </c>
-      <c r="O5" t="s">
+      <c r="B7" t="s">
+        <v>52</v>
+      </c>
+      <c r="C7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>50</v>
+      </c>
+      <c r="F7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" t="s">
+        <v>82</v>
+      </c>
+      <c r="I7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J7" s="1">
+        <v>44565</v>
+      </c>
+      <c r="K7" t="s">
+        <v>25</v>
+      </c>
+      <c r="L7" t="s">
+        <v>24</v>
+      </c>
+      <c r="M7" t="s">
+        <v>24</v>
+      </c>
+      <c r="N7" t="s">
+        <v>24</v>
+      </c>
+      <c r="O7" t="s">
+        <v>32</v>
+      </c>
+      <c r="P7" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" t="s">
         <v>44</v>
       </c>
-      <c r="P5" t="s">
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="Q5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17">
-      <c r="A6" t="s">
-        <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D6" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>55</v>
-      </c>
-      <c r="F6" t="s">
-        <v>22</v>
-      </c>
-      <c r="G6" t="s">
-        <v>22</v>
-      </c>
-      <c r="H6" t="s">
-        <v>56</v>
-      </c>
-      <c r="I6" t="s">
-        <v>24</v>
-      </c>
-      <c r="J6" t="s">
-        <v>57</v>
-      </c>
-      <c r="K6" t="s">
-        <v>26</v>
-      </c>
-      <c r="L6" t="s">
-        <v>24</v>
-      </c>
-      <c r="M6" t="s">
-        <v>24</v>
-      </c>
-      <c r="N6" t="s">
-        <v>24</v>
-      </c>
-      <c r="O6" t="s">
-        <v>24</v>
-      </c>
-      <c r="P6" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C7" t="s">
-        <v>39</v>
-      </c>
-      <c r="D7" t="s">
-        <v>49</v>
-      </c>
-      <c r="E7" t="s">
-        <v>55</v>
-      </c>
-      <c r="F7" t="s">
-        <v>42</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
-      </c>
-      <c r="H7" t="s">
-        <v>56</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7" t="s">
-        <v>60</v>
-      </c>
-      <c r="K7" t="s">
-        <v>26</v>
-      </c>
-      <c r="L7" t="s">
-        <v>24</v>
-      </c>
-      <c r="M7" t="s">
-        <v>24</v>
-      </c>
-      <c r="N7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O7" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" t="s">
-        <v>36</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17">
-      <c r="A8" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" t="s">
-        <v>49</v>
-      </c>
       <c r="E8" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G8" t="s">
         <v>23</v>
       </c>
       <c r="H8" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I8" t="s">
         <v>24</v>
       </c>
-      <c r="J8" t="s">
-        <v>63</v>
+      <c r="J8" s="1">
+        <v>44869</v>
       </c>
       <c r="K8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L8" t="s">
         <v>24</v>
@@ -1159,21 +1138,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="9" spans="1:17">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D9" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
         <v>22</v>
@@ -1188,10 +1167,10 @@
         <v>24</v>
       </c>
       <c r="J9" t="s">
-        <v>65</v>
+        <v>86</v>
       </c>
       <c r="K9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L9" t="s">
         <v>24</v>
@@ -1212,24 +1191,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:17">
+    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C10" t="s">
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E10" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F10" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G10" t="s">
         <v>22</v>
@@ -1241,10 +1220,10 @@
         <v>24</v>
       </c>
       <c r="J10" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="K10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L10" t="s">
         <v>24</v>
@@ -1265,21 +1244,21 @@
         <v>24</v>
       </c>
     </row>
-    <row r="11" spans="1:17">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="C11" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
         <v>22</v>
@@ -1288,16 +1267,16 @@
         <v>22</v>
       </c>
       <c r="H11" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I11" t="s">
         <v>24</v>
       </c>
       <c r="J11" t="s">
-        <v>69</v>
+        <v>87</v>
       </c>
       <c r="K11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L11" t="s">
         <v>24</v>
@@ -1318,39 +1297,39 @@
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:17">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>70</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G12" t="s">
         <v>23</v>
       </c>
       <c r="H12" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I12" t="s">
         <v>24</v>
       </c>
-      <c r="J12" t="s">
-        <v>72</v>
+      <c r="J12" s="1">
+        <v>44597</v>
       </c>
       <c r="K12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L12" t="s">
         <v>24</v>
@@ -1371,24 +1350,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:17">
+    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B13" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C13" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
         <v>22</v>
@@ -1400,10 +1379,10 @@
         <v>24</v>
       </c>
       <c r="J13" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="K13" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="L13" t="s">
         <v>24</v>
@@ -1424,39 +1403,39 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:17">
+    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="B14" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C14" t="s">
         <v>19</v>
       </c>
       <c r="D14" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E14" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="F14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G14" t="s">
         <v>22</v>
       </c>
       <c r="H14" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I14" t="s">
         <v>24</v>
       </c>
-      <c r="J14" t="s">
-        <v>60</v>
+      <c r="J14" s="1">
+        <v>44565</v>
       </c>
       <c r="K14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L14" t="s">
         <v>24</v>
@@ -1477,24 +1456,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:17">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E15" t="s">
         <v>21</v>
       </c>
       <c r="F15" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G15" t="s">
         <v>23</v>
@@ -1502,14 +1481,14 @@
       <c r="H15" s="1">
         <v>44624</v>
       </c>
-      <c r="I15" t="s">
-        <v>78</v>
+      <c r="I15" s="1">
+        <v>44745</v>
       </c>
       <c r="J15" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="K15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L15" t="s">
         <v>24</v>
@@ -1521,24 +1500,24 @@
         <v>24</v>
       </c>
       <c r="O15" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="P15" t="s">
-        <v>79</v>
+        <v>65</v>
       </c>
       <c r="Q15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="16" spans="1:17">
+    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C16" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D16" t="s">
         <v>20</v>
@@ -1547,25 +1526,25 @@
         <v>21</v>
       </c>
       <c r="F16" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G16" t="s">
         <v>22</v>
       </c>
       <c r="H16" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I16" t="s">
         <v>24</v>
       </c>
       <c r="J16" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="K16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L16" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="M16" t="s">
         <v>22</v>
@@ -1583,92 +1562,92 @@
         <v>24</v>
       </c>
     </row>
-    <row r="17" spans="1:17">
+    <row r="17" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>81</v>
+        <v>67</v>
       </c>
       <c r="B17" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F17" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G17" t="s">
         <v>22</v>
       </c>
       <c r="H17" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I17" t="s">
         <v>24</v>
       </c>
       <c r="J17" t="s">
+        <v>87</v>
+      </c>
+      <c r="K17" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" t="s">
+        <v>24</v>
+      </c>
+      <c r="M17" t="s">
+        <v>24</v>
+      </c>
+      <c r="N17" t="s">
+        <v>24</v>
+      </c>
+      <c r="O17" t="s">
+        <v>24</v>
+      </c>
+      <c r="P17" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>68</v>
+      </c>
+      <c r="B18" t="s">
+        <v>54</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+      <c r="D18" t="s">
+        <v>45</v>
+      </c>
+      <c r="E18" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" t="s">
         <v>69</v>
-      </c>
-      <c r="K17" t="s">
-        <v>26</v>
-      </c>
-      <c r="L17" t="s">
-        <v>24</v>
-      </c>
-      <c r="M17" t="s">
-        <v>24</v>
-      </c>
-      <c r="N17" t="s">
-        <v>24</v>
-      </c>
-      <c r="O17" t="s">
-        <v>24</v>
-      </c>
-      <c r="P17" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q17" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="1:17">
-      <c r="A18" t="s">
-        <v>82</v>
-      </c>
-      <c r="B18" t="s">
-        <v>62</v>
-      </c>
-      <c r="C18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D18" t="s">
-        <v>49</v>
-      </c>
-      <c r="E18" t="s">
-        <v>55</v>
-      </c>
-      <c r="F18" t="s">
-        <v>83</v>
       </c>
       <c r="G18" t="s">
         <v>23</v>
       </c>
       <c r="H18" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I18" t="s">
         <v>24</v>
       </c>
       <c r="J18" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="K18" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L18" t="s">
         <v>24</v>
@@ -1689,39 +1668,39 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:17">
+    <row r="19" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="B19" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E19" t="s">
         <v>21</v>
       </c>
       <c r="F19" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G19" t="s">
         <v>22</v>
       </c>
       <c r="H19" t="s">
-        <v>56</v>
-      </c>
-      <c r="I19" t="s">
-        <v>78</v>
-      </c>
-      <c r="J19" t="s">
-        <v>60</v>
+        <v>82</v>
+      </c>
+      <c r="I19" s="1">
+        <v>44745</v>
+      </c>
+      <c r="J19" s="1">
+        <v>44565</v>
       </c>
       <c r="K19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L19" t="s">
         <v>24</v>
@@ -1742,39 +1721,39 @@
         <v>24</v>
       </c>
     </row>
-    <row r="20" spans="1:17">
+    <row r="20" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B20" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D20" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E20" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F20" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G20" t="s">
         <v>23</v>
       </c>
       <c r="H20" t="s">
-        <v>56</v>
-      </c>
-      <c r="I20" t="s">
-        <v>78</v>
-      </c>
-      <c r="J20" t="s">
-        <v>60</v>
+        <v>82</v>
+      </c>
+      <c r="I20" s="1">
+        <v>44745</v>
+      </c>
+      <c r="J20" s="1">
+        <v>44565</v>
       </c>
       <c r="K20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L20" t="s">
         <v>24</v>
@@ -1792,24 +1771,24 @@
         <v>24</v>
       </c>
       <c r="Q20" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="21" spans="1:17">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>87</v>
+        <v>73</v>
       </c>
       <c r="B21" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C21" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D21" t="s">
         <v>20</v>
       </c>
       <c r="E21" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F21" t="s">
         <v>22</v>
@@ -1818,19 +1797,19 @@
         <v>22</v>
       </c>
       <c r="H21" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I21" t="s">
         <v>24</v>
       </c>
       <c r="J21" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="K21" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L21" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="M21" t="s">
         <v>22</v>
@@ -1848,39 +1827,39 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:17">
+    <row r="22" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="B22" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E22" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" t="s">
         <v>39</v>
       </c>
-      <c r="D22" t="s">
-        <v>40</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>42</v>
-      </c>
       <c r="G22" t="s">
         <v>22</v>
       </c>
       <c r="H22" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
       <c r="I22" t="s">
         <v>89</v>
       </c>
       <c r="J22" t="s">
-        <v>57</v>
+        <v>85</v>
       </c>
       <c r="K22" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="L22" t="s">
         <v>24</v>
@@ -1901,24 +1880,24 @@
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:17">
+    <row r="23" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
-        <v>90</v>
+        <v>75</v>
       </c>
       <c r="B23" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C23" t="s">
         <v>19</v>
       </c>
       <c r="D23" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="E23" t="s">
         <v>21</v>
       </c>
       <c r="F23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
         <v>23</v>
@@ -1927,28 +1906,28 @@
         <v>44630</v>
       </c>
       <c r="I23" t="s">
-        <v>74</v>
+        <v>88</v>
       </c>
       <c r="J23" t="s">
-        <v>43</v>
+        <v>83</v>
       </c>
       <c r="K23" t="s">
+        <v>25</v>
+      </c>
+      <c r="L23" t="s">
+        <v>24</v>
+      </c>
+      <c r="M23" t="s">
+        <v>24</v>
+      </c>
+      <c r="N23" t="s">
+        <v>24</v>
+      </c>
+      <c r="O23" t="s">
         <v>26</v>
       </c>
-      <c r="L23" t="s">
-        <v>24</v>
-      </c>
-      <c r="M23" t="s">
-        <v>24</v>
-      </c>
-      <c r="N23" t="s">
-        <v>24</v>
-      </c>
-      <c r="O23" t="s">
-        <v>28</v>
-      </c>
       <c r="P23" t="s">
-        <v>91</v>
+        <v>76</v>
       </c>
       <c r="Q23" t="s">
         <v>24</v>
@@ -1959,7 +1938,7 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:Q1 A16:Q17 A14:E14 G14:I14 A3:G3 A2:F2 I2:Q2 A6:Q7 A5:F5 I5:Q5 A11:Q11 A8:F8 H8:Q8 A13:G13 A12:F12 H12:Q12 A15:F15 A19:Q19 A18:F18 H18:Q18 A21:I21 A20:C20 H20:I20 A23:F23 I23:Q23 A4:G4 J4:Q4 I3:K3 J15:Q15 E20:F20 A22:H22 K22:Q22 A9:G9 I9:Q9 A10:G10 I10:Q10 I13:Q13 K21:Q21 K20:Q20 K14:Q14 M3:Q3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:K1 A17:G17 A14:E14 G14 A3:G3 A2:F2 I2 A7:G7 A5:F5 I5 A11:G11 A8:F8 I8 A13:G13 A12:F12 I12 A15:F15 A19:G19 A18:F18 I18 A21:G21 A20:C20 A23:F23 A4:G4 K4:Q4 I3 K15:Q15 E20:F20 A22:G22 K22:Q22 A9:G9 I9 A10:G10 I10 I13 K21 K20:Q20 K14:Q14 M3:Q3 A6:G6 I6 I7 I11 I14 A16:G16 I16 I17 I21 K2 K3 K5:Q5 K6:Q6 K7:Q7 K8:Q8 K9:Q9 K10:Q10 K11:Q11 K12:Q12 K13:Q13 K16 K17:Q17 K18:Q18 K19:Q19 K23:Q23 M2:Q2 M16:Q16 M21:Q21 M1:Q1" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1968,42 +1947,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.875" customWidth="1"/>
-    <col min="2" max="2" width="40.875" customWidth="1"/>
+    <col min="1" max="1" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>92</v>
+        <v>77</v>
       </c>
       <c r="B1" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>94</v>
+        <v>79</v>
       </c>
       <c r="B2" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>96</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>82</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:B3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:B2 A3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>